<commit_message>
# x-axis - time
</commit_message>
<xml_diff>
--- a/Weather Data_xlsx.xlsx
+++ b/Weather Data_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\PycharmProjects\Mathieu_Christian_Weather\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AE315135-E442-4E81-A7AD-4E37C317B62E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0414CF34-C430-4F5B-9227-D2218B591843}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2121,6 +2121,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="862363272"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2154,16 +2155,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2490,8 +2491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="X24" sqref="X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>